<commit_message>
Update pricing for new pulley
</commit_message>
<xml_diff>
--- a/Design/Pricing.xlsx
+++ b/Design/Pricing.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bsd405-my.sharepoint.com/personal/s-vikramadityan_bsd405_org/Documents/Tektite/TektiteR/EV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="141" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4E6A17E-DCB9-FA42-B233-BCDD7B8DF4A1}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFEAF77D-9B79-5541-A454-9A7789D1443C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Item</t>
   </si>
@@ -89,12 +89,6 @@
     <t>Motor pulley</t>
   </si>
   <si>
-    <t>https://www.aliexpress.us/item/3256803832945940.html</t>
-  </si>
-  <si>
-    <t>Potentially may get https://www.aliexpress.us/item/3256805934638435.html if it has bigger set screw</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.us/item/3256804652854836.html</t>
   </si>
   <si>
@@ -198,6 +192,9 @@
   </si>
   <si>
     <t>Getting 1 of the 5 in the JLCPCB order, added 3.58 of through hole components</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/3256805934638435.html</t>
   </si>
 </sst>
 </file>
@@ -302,6 +299,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -624,7 +625,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,12 +746,12 @@
         <v>14.874509999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C6" s="5">
         <f>1.98*1.101</f>
@@ -763,16 +764,13 @@
         <f t="shared" si="0"/>
         <v>2.17998</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="5">
         <f>3.54*1.101</f>
@@ -788,10 +786,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="5">
         <f>3.46*1.101</f>
@@ -807,10 +805,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="5">
         <f>0.8*1.101</f>
@@ -826,10 +824,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="5">
         <f>3.13*1.101</f>
@@ -845,10 +843,10 @@
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="5">
         <f>4.69*1.101</f>
@@ -863,15 +861,15 @@
         <v>3.098214</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C12" s="5">
         <f>1.101*5.02</f>
@@ -887,10 +885,10 @@
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="5">
         <f>2.75*1.101</f>
@@ -905,15 +903,15 @@
         <v>0.60555000000000003</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="5">
         <f>5.99*1.101</f>
@@ -928,15 +926,15 @@
         <v>0.92329860000000008</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" s="5">
         <f>8.69*1.101</f>
@@ -951,15 +949,15 @@
         <v>0.19135379999999999</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5">
         <f>8.09*1.01</f>
@@ -974,15 +972,15 @@
         <v>0.32683600000000002</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5">
         <f>11.98*1.101</f>
@@ -997,15 +995,15 @@
         <v>2.1983299999999999</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" s="5">
         <f>7.99*1.101</f>
@@ -1019,15 +1017,15 @@
         <v>0</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5">
         <f>(103.05 + 17.8)*1.101 + 3.58</f>
@@ -1042,15 +1040,15 @@
         <v>27.327170000000002</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" s="5">
         <f>3.25*1.101</f>

</xml_diff>

<commit_message>
Update pricing with real-world orders
</commit_message>
<xml_diff>
--- a/Design/Pricing.xlsx
+++ b/Design/Pricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bsd405-my.sharepoint.com/personal/s-vikramadityan_bsd405_org/Documents/Tektite/TektiteR/EV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CFEAF77D-9B79-5541-A454-9A7789D1443C}"/>
+  <xr:revisionPtr revIDLastSave="165" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1587D249-BE70-0D46-A5D6-DAC8FECD2543}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
   </bookViews>
@@ -98,15 +98,9 @@
     <t>Short belt pulley (20T5-60T5, 2GT-158-6)</t>
   </si>
   <si>
-    <t>Central shaft</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.us/item/3256806106856975.html</t>
   </si>
   <si>
-    <t>Wheel D shaft</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.us/item/3256806188242363.html</t>
   </si>
   <si>
@@ -195,6 +189,12 @@
   </si>
   <si>
     <t>https://www.aliexpress.us/item/3256805934638435.html</t>
+  </si>
+  <si>
+    <t>Wheel D shaft (5x138mm)</t>
+  </si>
+  <si>
+    <t>Central shaft (5mm diameter, 100mm long)</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,7 +663,7 @@
       </c>
       <c r="H1" s="6">
         <f>SUM(E:E)</f>
-        <v>106.94254034090001</v>
+        <v>109.18848034089999</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -735,15 +735,15 @@
         <v>15</v>
       </c>
       <c r="C5" s="5">
-        <f>13.51*1.101</f>
-        <v>14.874509999999999</v>
+        <f>16.62*1.101</f>
+        <v>18.29862</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>14.874509999999999</v>
+        <v>18.29862</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -751,7 +751,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" s="5">
         <f>1.98*1.101</f>
@@ -805,10 +805,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="C9" s="5">
         <f>0.8*1.101</f>
@@ -824,10 +824,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5">
         <f>3.13*1.101</f>
@@ -843,10 +843,10 @@
     </row>
     <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5">
         <f>4.69*1.101</f>
@@ -861,15 +861,15 @@
         <v>3.098214</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C12" s="5">
         <f>1.101*5.02</f>
@@ -885,10 +885,10 @@
     </row>
     <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C13" s="5">
         <f>2.75*1.101</f>
@@ -903,15 +903,15 @@
         <v>0.60555000000000003</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5">
         <f>5.99*1.101</f>
@@ -926,15 +926,15 @@
         <v>0.92329860000000008</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5">
         <f>8.69*1.101</f>
@@ -949,15 +949,15 @@
         <v>0.19135379999999999</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16" s="5">
         <f>8.09*1.01</f>
@@ -972,15 +972,15 @@
         <v>0.32683600000000002</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" s="5">
         <f>11.98*1.101</f>
@@ -995,15 +995,15 @@
         <v>2.1983299999999999</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5">
         <f>7.99*1.101</f>
@@ -1017,19 +1017,19 @@
         <v>0</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5">
-        <f>(103.05 + 17.8)*1.101 + 3.58</f>
-        <v>136.63585</v>
+        <f>123.93 + 3.58</f>
+        <v>127.51</v>
       </c>
       <c r="D19" s="9">
         <f>1/5</f>
@@ -1037,29 +1037,29 @@
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
-        <v>27.327170000000002</v>
+        <v>25.502000000000002</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="5">
-        <f>3.25*1.101</f>
-        <v>3.5782499999999997</v>
+        <v>74.8</v>
       </c>
       <c r="D20" s="9">
-        <v>4</v>
+        <f>4/20</f>
+        <v>0.2</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>14.312999999999999</v>
+        <v>14.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update pricing and remove debug print
</commit_message>
<xml_diff>
--- a/Design/Pricing.xlsx
+++ b/Design/Pricing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bsd405-my.sharepoint.com/personal/s-vikramadityan_bsd405_org/Documents/Tektite/TektiteR/EV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="165" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1587D249-BE70-0D46-A5D6-DAC8FECD2543}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA9B8474-CA16-BE4D-9075-7096C4274EBA}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Item</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Black PLA</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/dp/B0BV24T11D/</t>
   </si>
   <si>
@@ -122,33 +119,18 @@
     <t>https://www.aliexpress.us/item/3256804650896588.html</t>
   </si>
   <si>
-    <t>Encoder JST connector (PH 2mm, 4P)</t>
-  </si>
-  <si>
     <t>Comes in pack of 5</t>
   </si>
   <si>
-    <t>Short screw</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/dp/B012TE12CY</t>
   </si>
   <si>
-    <t>Need 14/100 screws</t>
-  </si>
-  <si>
-    <t>MP screw</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/dp/B07MHNXPJL</t>
   </si>
   <si>
     <t>Need 2/100 screws</t>
   </si>
   <si>
-    <t>Wheel screw</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/dp/B01BBOZ4JA/</t>
   </si>
   <si>
@@ -185,9 +167,6 @@
     <t>BaneBots Wheels</t>
   </si>
   <si>
-    <t>Getting 1 of the 5 in the JLCPCB order, added 3.58 of through hole components</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.us/item/3256805934638435.html</t>
   </si>
   <si>
@@ -195,6 +174,33 @@
   </si>
   <si>
     <t>Central shaft (5mm diameter, 100mm long)</t>
+  </si>
+  <si>
+    <t>Encoder JST connector (PH 2mm, 4P) + Heatshrink</t>
+  </si>
+  <si>
+    <t>Need 17/100 screws</t>
+  </si>
+  <si>
+    <t>Short screw (M3x6mmm)</t>
+  </si>
+  <si>
+    <t>MP screw (M3x12mm)</t>
+  </si>
+  <si>
+    <t>Wheel screw (M3x16mm)</t>
+  </si>
+  <si>
+    <t>Getting 1 of the 10 in the JLCPCB order</t>
+  </si>
+  <si>
+    <t>Black PLA (Frame)</t>
+  </si>
+  <si>
+    <t>Thank You note</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -622,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DC6279-EE2D-524A-AEA0-F780B55F0CE3}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" customWidth="1"/>
+    <col min="1" max="1" width="41.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" style="5"/>
     <col min="4" max="4" width="10.83203125" style="9"/>
@@ -663,15 +669,15 @@
       </c>
       <c r="H1" s="6">
         <f>SUM(E:E)</f>
-        <v>109.18848034089999</v>
+        <v>104.5133300409</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="5">
         <f>47.96*1.101</f>
@@ -688,401 +694,419 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5">
+        <f>16.62*1.101</f>
+        <v>18.29862</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <f>C3*D3</f>
+        <v>18.29862</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5">
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5">
         <f>8.48*1.101</f>
         <v>9.3364799999999999</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D4" s="9">
         <v>0.5</v>
       </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E20" si="0">C3*D3</f>
+      <c r="E4" s="5">
+        <f t="shared" ref="E4:E21" si="0">C4*D4</f>
         <v>4.6682399999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5">
+        <v>74.8</v>
+      </c>
+      <c r="D5" s="9">
+        <f>4/20</f>
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="5">
+        <f>C5*D5</f>
+        <v>14.96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5">
+        <f>0.8*1.101</f>
+        <v>0.88080000000000003</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <f>C6*D6</f>
+        <v>0.88080000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="5">
+        <f>3.13*1.101</f>
+        <v>3.4461299999999997</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5">
+        <f>C7*D7</f>
+        <v>6.8922599999999994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="C8" s="5">
         <f>(6.5 + 5.26/2)*1.101</f>
         <v>10.052129999999998</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D8" s="9">
         <v>1</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E8" s="5">
         <f t="shared" si="0"/>
         <v>10.052129999999998</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="F8" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5">
-        <f>16.62*1.101</f>
-        <v>18.29862</v>
-      </c>
-      <c r="D5" s="9">
-        <v>1</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>18.29862</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5">
         <f>1.98*1.101</f>
         <v>2.17998</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D9" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E9" s="5">
         <f t="shared" si="0"/>
         <v>2.17998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="5">
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="5">
         <f>3.54*1.101</f>
         <v>3.8975399999999998</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D10" s="9">
         <v>2</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>7.7950799999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="5">
         <f>3.46*1.101</f>
         <v>3.8094600000000001</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D11" s="9">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
         <v>3.8094600000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="5">
-        <f>0.8*1.101</f>
-        <v>0.88080000000000003</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.88080000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="7" t="s">
+    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5">
-        <f>3.13*1.101</f>
-        <v>3.4461299999999997</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>6.8922599999999994</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="C12" s="5">
         <f>4.69*1.101</f>
         <v>5.1636899999999999</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D12" s="9">
         <f>6/10</f>
         <v>0.6</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
         <f t="shared" si="0"/>
         <v>3.098214</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F12" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="C13" s="5">
         <f>1.101*5.02</f>
         <v>5.5270199999999994</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D13" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E13" s="5">
         <f t="shared" si="0"/>
         <v>5.5270199999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="5">
+    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="5">
         <f>2.75*1.101</f>
         <v>3.0277500000000002</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D14" s="9">
         <f>1/5</f>
         <v>0.2</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E14" s="5">
         <f t="shared" si="0"/>
         <v>0.60555000000000003</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="F14" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="5">
         <f>5.99*1.101</f>
         <v>6.5949900000000001</v>
       </c>
-      <c r="D14" s="9">
-        <f>14/100</f>
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.92329860000000008</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="D15" s="9">
+        <f>17/100</f>
+        <v>0.17</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1211483000000002</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="5">
         <f>8.69*1.101</f>
         <v>9.5676899999999989</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D16" s="9">
         <f>2/100</f>
         <v>0.02</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E16" s="5">
         <f t="shared" si="0"/>
         <v>0.19135379999999999</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="F16" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="5">
         <f>8.09*1.01</f>
         <v>8.1708999999999996</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D17" s="9">
         <f>4/100</f>
         <v>0.04</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E17" s="5">
         <f t="shared" si="0"/>
         <v>0.32683600000000002</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="F17" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5">
         <f>11.98*1.101</f>
         <v>13.18998</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D18" s="9">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E18" s="5">
         <f t="shared" si="0"/>
         <v>2.1983299999999999</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="F18" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="5">
         <f>7.99*1.101</f>
         <v>8.7969899999999992</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D19" s="9">
         <v>0</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="5">
-        <f>123.93 + 3.58</f>
-        <v>127.51</v>
-      </c>
-      <c r="D19" s="9">
-        <f>1/5</f>
-        <v>0.2</v>
-      </c>
-      <c r="E19" s="5">
-        <f t="shared" si="0"/>
-        <v>25.502000000000002</v>
-      </c>
       <c r="F19" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C20" s="5">
-        <v>74.8</v>
+        <f>206.29</f>
+        <v>206.29</v>
       </c>
       <c r="D20" s="9">
-        <f>4/20</f>
-        <v>0.2</v>
+        <f>1/10</f>
+        <v>0.1</v>
       </c>
       <c r="E20" s="5">
         <f t="shared" si="0"/>
-        <v>14.96</v>
+        <v>20.629000000000001</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="5">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{1127F7E8-945F-6540-8786-B8DD605BE466}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{D3B435A3-CA86-464A-A059-1F86BC2B6302}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{56DFB920-5C58-D642-A245-6E447AD57C46}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{B04138BF-1945-6A41-A50E-E8C23A6D1AE8}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{836360E0-2B7D-0243-9771-1A769D84D753}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{EA9A5D7F-69A1-6E4E-80E7-ECD779D7D388}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{A98E6176-4710-9C49-9972-B7FAAC6C040A}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{D018B163-F347-D142-8B31-E5E0A887A9EB}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{BF251B86-54EE-234C-A5E5-3A707CBCBCD2}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{1C48D52B-8F5E-444E-BB19-F4A375B6DD01}"/>
-    <hyperlink ref="B12" r:id="rId11" xr:uid="{0E06D031-7BD1-544D-8989-1A3139BD38D8}"/>
-    <hyperlink ref="B13" r:id="rId12" xr:uid="{9D4094F4-F98A-6344-810A-A3F71068A0C8}"/>
-    <hyperlink ref="B14" r:id="rId13" xr:uid="{B6AF7F62-C552-5948-9DFD-EE421B26F3A5}"/>
-    <hyperlink ref="B15" r:id="rId14" xr:uid="{B79725FD-8953-2642-9D3D-B936199B0B2B}"/>
-    <hyperlink ref="B16" r:id="rId15" xr:uid="{CD47833C-856A-834C-B374-62C8E153EBEB}"/>
-    <hyperlink ref="B17" r:id="rId16" xr:uid="{D94F7B8F-31F0-4D48-95E1-72495218D91B}"/>
-    <hyperlink ref="B18" r:id="rId17" xr:uid="{D46D8567-27E0-4A47-B972-5C7384A23E5C}"/>
-    <hyperlink ref="B19" r:id="rId18" xr:uid="{B251EDFF-D916-5B47-9C82-AE2C63A918C4}"/>
-    <hyperlink ref="B20" r:id="rId19" xr:uid="{32EA09CA-016F-3D43-A8B7-94E4B11169EF}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{D3B435A3-CA86-464A-A059-1F86BC2B6302}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{56DFB920-5C58-D642-A245-6E447AD57C46}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{B04138BF-1945-6A41-A50E-E8C23A6D1AE8}"/>
+    <hyperlink ref="B9" r:id="rId4" xr:uid="{836360E0-2B7D-0243-9771-1A769D84D753}"/>
+    <hyperlink ref="B10" r:id="rId5" xr:uid="{EA9A5D7F-69A1-6E4E-80E7-ECD779D7D388}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{A98E6176-4710-9C49-9972-B7FAAC6C040A}"/>
+    <hyperlink ref="B6" r:id="rId7" xr:uid="{D018B163-F347-D142-8B31-E5E0A887A9EB}"/>
+    <hyperlink ref="B7" r:id="rId8" xr:uid="{BF251B86-54EE-234C-A5E5-3A707CBCBCD2}"/>
+    <hyperlink ref="B12" r:id="rId9" xr:uid="{1C48D52B-8F5E-444E-BB19-F4A375B6DD01}"/>
+    <hyperlink ref="B13" r:id="rId10" xr:uid="{0E06D031-7BD1-544D-8989-1A3139BD38D8}"/>
+    <hyperlink ref="B14" r:id="rId11" xr:uid="{9D4094F4-F98A-6344-810A-A3F71068A0C8}"/>
+    <hyperlink ref="B15" r:id="rId12" xr:uid="{B6AF7F62-C552-5948-9DFD-EE421B26F3A5}"/>
+    <hyperlink ref="B16" r:id="rId13" xr:uid="{B79725FD-8953-2642-9D3D-B936199B0B2B}"/>
+    <hyperlink ref="B17" r:id="rId14" xr:uid="{CD47833C-856A-834C-B374-62C8E153EBEB}"/>
+    <hyperlink ref="B18" r:id="rId15" xr:uid="{D94F7B8F-31F0-4D48-95E1-72495218D91B}"/>
+    <hyperlink ref="B19" r:id="rId16" xr:uid="{D46D8567-27E0-4A47-B972-5C7384A23E5C}"/>
+    <hyperlink ref="B20" r:id="rId17" xr:uid="{B251EDFF-D916-5B47-9C82-AE2C63A918C4}"/>
+    <hyperlink ref="B5" r:id="rId18" xr:uid="{32EA09CA-016F-3D43-A8B7-94E4B11169EF}"/>
+    <hyperlink ref="B2" r:id="rId19" xr:uid="{1127F7E8-945F-6540-8786-B8DD605BE466}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update pricing, make text more reliable
</commit_message>
<xml_diff>
--- a/Design/Pricing.xlsx
+++ b/Design/Pricing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bsd405-my.sharepoint.com/personal/s-vikramadityan_bsd405_org/Documents/Tektite/TektiteR/EV/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA9B8474-CA16-BE4D-9075-7096C4274EBA}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{355650BB-0AA2-E14E-AC49-163D93A781F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28D3C3E8-BCE7-3541-B729-90A9B49BE73C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{3323777E-1DF2-4348-B326-362B318325C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>Item</t>
   </si>
@@ -107,9 +107,6 @@
     <t>https://www.aliexpress.us/item/3256806307993875.html</t>
   </si>
   <si>
-    <t>Need 6 bearing, comes in lot of 10</t>
-  </si>
-  <si>
     <t>Quadrature encoder</t>
   </si>
   <si>
@@ -201,6 +198,33 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>Alternate: https://www.aliexpress.us/item/3256807041239789.html</t>
+  </si>
+  <si>
+    <t>Alternate: https://www.aliexpress.us/item/3256805329452853.html</t>
+  </si>
+  <si>
+    <t>Alternate: https://www.aliexpress.us/item/3256803888885845.html</t>
+  </si>
+  <si>
+    <t>Alternate: https://www.aliexpress.us/item/3256802203384432.html and https://www.aliexpress.us/item/2251832693571771.html</t>
+  </si>
+  <si>
+    <t>Need 6 bearing, comes in lot of 10, Alternate: https://www.aliexpress.us/item/3256805156145762.html</t>
+  </si>
+  <si>
+    <t>Button caps</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.us/item/2251832666419248.html</t>
+  </si>
+  <si>
+    <t> $              5.71 </t>
+  </si>
+  <si>
+    <t> $              0.11 </t>
   </si>
 </sst>
 </file>
@@ -210,7 +234,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -240,6 +264,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -264,7 +294,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -287,6 +317,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -628,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DC6279-EE2D-524A-AEA0-F780B55F0CE3}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="165" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,12 +701,12 @@
       </c>
       <c r="H1" s="6">
         <f>SUM(E:E)</f>
-        <v>104.5133300409</v>
+        <v>103.91333004089999</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>7</v>
@@ -692,7 +724,7 @@
         <v>1.2793079408999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -710,6 +742,9 @@
         <f>C3*D3</f>
         <v>18.29862</v>
       </c>
+      <c r="F3" s="11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -726,16 +761,16 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E21" si="0">C4*D4</f>
+        <f t="shared" ref="E4:E22" si="0">C4*D4</f>
         <v>4.6682399999999999</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5">
         <v>74.8</v>
@@ -751,7 +786,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>19</v>
@@ -770,7 +805,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>20</v>
@@ -809,12 +844,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="5">
         <f>1.98*1.101</f>
@@ -827,8 +862,11 @@
         <f t="shared" si="0"/>
         <v>2.17998</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F9" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -846,8 +884,11 @@
         <f t="shared" si="0"/>
         <v>7.7950799999999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F10" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="85" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -865,8 +906,11 @@
         <f t="shared" si="0"/>
         <v>3.8094600000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="F11" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -886,15 +930,15 @@
         <v>3.098214</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>25</v>
       </c>
       <c r="C13" s="5">
         <f>1.101*5.02</f>
@@ -910,10 +954,10 @@
     </row>
     <row r="14" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="5">
         <f>2.75*1.101</f>
@@ -928,15 +972,15 @@
         <v>0.60555000000000003</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="5">
         <f>5.99*1.101</f>
@@ -951,15 +995,15 @@
         <v>1.1211483000000002</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5">
         <f>8.69*1.101</f>
@@ -974,114 +1018,132 @@
         <v>0.19135379999999999</v>
       </c>
       <c r="F16" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="5">
+      <c r="C18" s="5">
         <f>8.09*1.01</f>
         <v>8.1708999999999996</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D18" s="9">
         <f>4/100</f>
         <v>0.04</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E18" s="5">
         <f t="shared" si="0"/>
         <v>0.32683600000000002</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F18" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="C19" s="5">
         <f>11.98*1.101</f>
         <v>13.18998</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D19" s="9">
         <f>1/6</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E19" s="5">
         <f t="shared" si="0"/>
         <v>2.1983299999999999</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F19" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="5">
+      <c r="C20" s="5">
         <f>7.99*1.101</f>
         <v>8.7969899999999992</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D20" s="9">
         <v>0</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F20" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="B21" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="5">
-        <f>206.29</f>
-        <v>206.29</v>
-      </c>
-      <c r="D20" s="9">
+      <c r="C21" s="5">
+        <f>206.29-6</f>
+        <v>200.29</v>
+      </c>
+      <c r="D21" s="9">
         <f>1/10</f>
         <v>0.1</v>
       </c>
-      <c r="E20" s="5">
-        <f t="shared" si="0"/>
-        <v>20.629000000000001</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>20.029</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="C22" s="5">
         <v>0</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D22" s="9">
         <v>1</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1101,13 +1163,15 @@
     <hyperlink ref="B14" r:id="rId11" xr:uid="{9D4094F4-F98A-6344-810A-A3F71068A0C8}"/>
     <hyperlink ref="B15" r:id="rId12" xr:uid="{B6AF7F62-C552-5948-9DFD-EE421B26F3A5}"/>
     <hyperlink ref="B16" r:id="rId13" xr:uid="{B79725FD-8953-2642-9D3D-B936199B0B2B}"/>
-    <hyperlink ref="B17" r:id="rId14" xr:uid="{CD47833C-856A-834C-B374-62C8E153EBEB}"/>
-    <hyperlink ref="B18" r:id="rId15" xr:uid="{D94F7B8F-31F0-4D48-95E1-72495218D91B}"/>
-    <hyperlink ref="B19" r:id="rId16" xr:uid="{D46D8567-27E0-4A47-B972-5C7384A23E5C}"/>
-    <hyperlink ref="B20" r:id="rId17" xr:uid="{B251EDFF-D916-5B47-9C82-AE2C63A918C4}"/>
+    <hyperlink ref="B18" r:id="rId14" xr:uid="{CD47833C-856A-834C-B374-62C8E153EBEB}"/>
+    <hyperlink ref="B19" r:id="rId15" xr:uid="{D94F7B8F-31F0-4D48-95E1-72495218D91B}"/>
+    <hyperlink ref="B20" r:id="rId16" xr:uid="{D46D8567-27E0-4A47-B972-5C7384A23E5C}"/>
+    <hyperlink ref="B21" r:id="rId17" xr:uid="{B251EDFF-D916-5B47-9C82-AE2C63A918C4}"/>
     <hyperlink ref="B5" r:id="rId18" xr:uid="{32EA09CA-016F-3D43-A8B7-94E4B11169EF}"/>
     <hyperlink ref="B2" r:id="rId19" xr:uid="{1127F7E8-945F-6540-8786-B8DD605BE466}"/>
+    <hyperlink ref="B17" r:id="rId20" xr:uid="{6E79EDA6-ED52-C547-99A7-BFAFBAB2AE0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>